<commit_message>
added articles Schneider, Mako, Sever
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -49,6 +49,27 @@
   </si>
   <si>
     <t>sever</t>
+  </si>
+  <si>
+    <t>sever - longtable</t>
+  </si>
+  <si>
+    <t>schneider</t>
+  </si>
+  <si>
+    <t>schneider tabs</t>
+  </si>
+  <si>
+    <t>schneider images + text</t>
+  </si>
+  <si>
+    <t>tiraz + submission</t>
+  </si>
+  <si>
+    <t>Funta + Mako lit</t>
+  </si>
+  <si>
+    <t>Sever lit</t>
   </si>
 </sst>
 </file>
@@ -428,7 +449,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="0">D5-C5</f>
+        <f t="shared" ref="F5:F22" si="0">D5-C5</f>
         <v>1.736111111111116E-2</v>
       </c>
       <c r="H5" s="7"/>
@@ -705,8 +726,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.89930555555555547</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -720,10 +740,22 @@
       <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="B13" s="2">
+        <v>41986</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333326</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="9"/>
@@ -737,9 +769,19 @@
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="3">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="9"/>
@@ -753,9 +795,19 @@
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="3">
+        <v>0.89236111111111116</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.90625</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="9"/>
@@ -769,9 +821,18 @@
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="3">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="3">
+        <v>6.25E-2</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="9"/>
@@ -784,10 +845,22 @@
       <c r="Q16" s="8"/>
     </row>
     <row r="17" spans="2:17">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="B17" s="2">
+        <v>41987</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>5.208333333333337E-2</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="9"/>
@@ -801,9 +874,19 @@
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="C18" s="3">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -817,9 +900,19 @@
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="3">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>4.861111111111116E-2</v>
+      </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -833,9 +926,19 @@
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="3">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="9"/>
@@ -849,9 +952,19 @@
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="3">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>4.513888888888884E-2</v>
+      </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="9"/>
@@ -865,9 +978,19 @@
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="3">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333336E-2</v>
+      </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="9"/>

</xml_diff>